<commit_message>
Finalized project plan + updated readme
</commit_message>
<xml_diff>
--- a/project-management.xlsx
+++ b/project-management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bertelsmann-my.sharepoint.com/personal/soenke_broihan_bertelsmann_de/Documents/Udacity-DevOps/project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bertelsmann-my.sharepoint.com/personal/soenke_broihan_bertelsmann_de/Documents/Udacity-DevOps/project2/flask-ml-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{56D4ACAD-222C-43D8-A0FC-943F8040A70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29428B0B-DE10-4B34-98E3-4EE242A364CF}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{56D4ACAD-222C-43D8-A0FC-943F8040A70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F72F34D-7597-4B4F-9EB3-F1781604960B}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>Week</t>
   </si>
@@ -103,6 +103,47 @@
   <si>
     <t>Add more automated testing</t>
   </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Q3 2023</t>
+  </si>
+  <si>
+    <t>Q4 2023</t>
+  </si>
+  <si>
+    <t>Q1 2024</t>
+  </si>
+  <si>
+    <t>Q2 2024</t>
+  </si>
+  <si>
+    <t>Extend the API to make the prediction model selectable from the REST request</t>
+  </si>
+  <si>
+    <t>Enhance the UI to support making prediction from the homepage with user input</t>
+  </si>
+  <si>
+    <t>Automate infrastructure setup using terraform</t>
+  </si>
+  <si>
+    <t>Support uploading of prediction models and allow "abstract" prediction Request</t>
+  </si>
+  <si>
+    <t>Support uploading prediction models and "abstract" prediciton Requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make infrastructure scalable </t>
+  </si>
+  <si>
+    <t>Have a more or less generic backend supporting an prediction models and
+user input variables for the prediction model</t>
+  </si>
+  <si>
+    <t>Have a very handy web gui to work with any given prediction model and custom 
+input variables for that model</t>
+  </si>
 </sst>
 </file>
 
@@ -175,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -191,6 +232,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -412,7 +456,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29572,14 +29616,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06569FED-4055-47B2-BA5B-741D58BC2E10}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="66.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>